<commit_message>
Got it! Sth. wrong in ufd prf functions. That is deltax_deltay vec has been modified.
</commit_message>
<xml_diff>
--- a/config/cfg_ufd/c_cof_1580.xlsx
+++ b/config/cfg_ufd/c_cof_1580.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\板形计算\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digestion\tiny_ssu_calc\config\cfg_ufd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20670" windowHeight="10065"/>
+    <workbookView xWindow="935" yWindow="0" windowWidth="20665" windowHeight="10069"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,17 +392,17 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="12.625" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
-    <col min="11" max="11" width="22.125" customWidth="1"/>
+    <col min="2" max="9" width="12.59765625" customWidth="1"/>
+    <col min="10" max="10" width="12.69921875" customWidth="1"/>
+    <col min="11" max="11" width="22.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>-1.2923691E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -486,7 +486,7 @@
         <v>-8.4320651999999997E-13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -515,7 +515,7 @@
         <v>5.7777059000000002E-11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -544,7 +544,7 @@
         <v>1.0165365999999999E-11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -573,7 +573,7 @@
         <v>-2.2757952000000001E-12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -602,7 +602,7 @@
         <v>-1.0494234E-13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -631,7 +631,7 @@
         <v>-3.6405046999999998E-16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
         <v>9.3344713999999998E-17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -689,7 +689,7 @@
         <v>8.3765416999999999E-12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1.1798418E-13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -747,7 +747,7 @@
         <v>1.1151474E-16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -776,7 +776,7 @@
         <v>8.8151813000000002E-16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -805,7 +805,7 @@
         <v>2.5804669000000001E-17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -834,7 +834,7 @@
         <v>9.9622675999999994E-20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -863,7 +863,7 @@
         <v>-9.3077725000000005E-14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -892,7 +892,7 @@
         <v>-5.5767750999999998E-17</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -921,7 +921,7 @@
         <v>-8.5358330000000001E-17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>

</xml_diff>